<commit_message>
add DS18B20 temp sensor, cmd from serial
</commit_message>
<xml_diff>
--- a/doc/growmat_easy.xlsx
+++ b/doc/growmat_easy.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="24120" windowHeight="14460"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="24120" windowHeight="14460" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="price list" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="growmat_easy_hydro" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="110">
   <si>
     <t>box</t>
   </si>
@@ -198,6 +198,153 @@
   </si>
   <si>
     <t>prace 3h?</t>
+  </si>
+  <si>
+    <t>433MHz socket</t>
+  </si>
+  <si>
+    <t>keyboard</t>
+  </si>
+  <si>
+    <t>arduino mega</t>
+  </si>
+  <si>
+    <t>battery</t>
+  </si>
+  <si>
+    <t>charger</t>
+  </si>
+  <si>
+    <t>433MHz tx</t>
+  </si>
+  <si>
+    <t>dc step-up</t>
+  </si>
+  <si>
+    <t>gsm</t>
+  </si>
+  <si>
+    <t>ph probe</t>
+  </si>
+  <si>
+    <t>ph modul</t>
+  </si>
+  <si>
+    <t>ec probe</t>
+  </si>
+  <si>
+    <t>ec modul</t>
+  </si>
+  <si>
+    <t>thermo/humidyty meter air</t>
+  </si>
+  <si>
+    <t>light sensor</t>
+  </si>
+  <si>
+    <t>thermometer water</t>
+  </si>
+  <si>
+    <t>ultrasonic distance meter</t>
+  </si>
+  <si>
+    <t>level switch</t>
+  </si>
+  <si>
+    <t>usb cable</t>
+  </si>
+  <si>
+    <t>power source</t>
+  </si>
+  <si>
+    <t>coeficient</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>descr</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>http://www.giganto.cz/elektronika/dalkove-ovladane-bezdratove-zasuvky-3600w</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>cz</t>
+  </si>
+  <si>
+    <t>vat</t>
+  </si>
+  <si>
+    <t>https://www.postavrobota.cz/Vysilac-433MHz-ASK-antena-d663.htm</t>
+  </si>
+  <si>
+    <t>https://www.postavrobota.cz/I2C-LCD-displej-znakovy-16x2-modry-d333.htm</t>
+  </si>
+  <si>
+    <t>https://www.postavrobota.cz/Membranova-klavesnice-4x3-samolepici-d137.htm</t>
+  </si>
+  <si>
+    <t>http://www.ebay.com/itm/PCF8574-PCF8574T-I2C-8-Bit-IO-GPIO-Expander-Module-for-Arduino-Raspberry-Pi-UK-/272432637606?var=&amp;hash=item3f6e4026a6:m:mQFPRLxSj-zVxa61Qe6YVhQ</t>
+  </si>
+  <si>
+    <t>ebay</t>
+  </si>
+  <si>
+    <t>https://www.postavrobota.cz/Dccduino-Mega-ATmega2560-Arduino-kompatibilni-d100.htm</t>
+  </si>
+  <si>
+    <t>https://www.postavrobota.cz/Mini-nabijecka-Li-ion-Li-po-clanku-s-ochranou-baterie-d10.htm</t>
+  </si>
+  <si>
+    <t>https://www.postavrobota.cz/RTC-modul-realneho-casu-DS1307-baterie-d123.htm</t>
+  </si>
+  <si>
+    <t>https://www.postavrobota.cz/Mini-nastavitelny-zdroj-zvysujici-napeti-2A-d136.htm</t>
+  </si>
+  <si>
+    <t>ec dc-dc isolated</t>
+  </si>
+  <si>
+    <t>pcb ps</t>
+  </si>
+  <si>
+    <t>pcb ec</t>
+  </si>
+  <si>
+    <t>pcb ?</t>
+  </si>
+  <si>
+    <t>https://www.postavrobota.cz/DC-DC-5V-5V-izolovany-zdroj-1W-d279.htm</t>
+  </si>
+  <si>
+    <t>https://www.postavrobota.cz/Digitalni-teplotni-sonda-DS18B20-2m-d370.htm</t>
+  </si>
+  <si>
+    <t>http://www.ebay.com/itm/SIM800L-GPRS-GSM-SIM-Board-Quadband-QUAD-BAND-L-shape-Antenna-for-Arduino-/281958541036?hash=item41a609e6ec:g:5JUAAOSwMVdYFv3B</t>
+  </si>
+  <si>
+    <t>http://www.ebay.com/itm/Liquid-PH0-14-Value-Detect-Sensor-Module-PH-Electrode-Probe-BNC-for-Arduino-G-/262617141991?hash=item3d253392e7:g:T0IAAOSwxg5X0kt3</t>
+  </si>
+  <si>
+    <t>http://www.ebay.com/itm/E201WM-Conductivity-COND-EC-electrode-Conductivity-sensor-probe-BNC-connector-/141936907599?hash=item210c19554f:g:eRUAAOSwEK9Txo38</t>
+  </si>
+  <si>
+    <t>http://www.ebay.com/itm/4pcs-3-7V-18650-9900mah-Li-ion-Rechargeable-Battery-For-LED-Flashlight-Torch-LO-/161933546105?hash=item25b3fdd279:g:JuIAAOSwZG9WhJCM</t>
+  </si>
+  <si>
+    <t>http://www.ebay.com/itm/Ultrasonic-Module-Distance-Measuring-Transducer-Sensor-Waterproof-Perfect-/272041782549?hash=item3f56f42d15:g:mMYAAOSw5ZBWQbkT</t>
+  </si>
+  <si>
+    <t>esp8266</t>
+  </si>
+  <si>
+    <t>https://www.postavrobota.cz/WiFi-RS232-AT-modul-ESP8266-2-4GHz-SoC-d159.htm</t>
   </si>
 </sst>
 </file>
@@ -914,8 +1061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1747,12 +1894,1079 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B1:M46"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J1" t="s">
+        <v>87</v>
+      </c>
+      <c r="L1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>280</v>
+      </c>
+      <c r="E3">
+        <f>D3*C3</f>
+        <v>280</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <f>F3*E3</f>
+        <v>280</v>
+      </c>
+      <c r="I3" t="s">
+        <v>86</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="M3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>700</v>
+      </c>
+      <c r="E4">
+        <f>D4*C4</f>
+        <v>700</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <f>F4*E4</f>
+        <v>700</v>
+      </c>
+      <c r="I4" t="s">
+        <v>86</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="M4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>40</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E5:E37" si="0">D5*C5</f>
+        <v>40</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ref="G5:G37" si="1">F5*E5</f>
+        <v>40</v>
+      </c>
+      <c r="I5" t="s">
+        <v>86</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>160</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="I6" t="s">
+        <v>86</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>40</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="I7" t="s">
+        <v>86</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>50</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="I8" t="s">
+        <v>92</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>400</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>400</v>
+      </c>
+      <c r="I9" t="s">
+        <v>86</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="M9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>50</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="I10" t="s">
+        <v>92</v>
+      </c>
+      <c r="M10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>45</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="I11" t="s">
+        <v>86</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="M11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>35</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="I12" t="s">
+        <v>86</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="M12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>300</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>600</v>
+      </c>
+      <c r="I13" t="s">
+        <v>92</v>
+      </c>
+      <c r="M13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>700</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>700</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>1400</v>
+      </c>
+      <c r="I14" t="s">
+        <v>92</v>
+      </c>
+      <c r="M14" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>700</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>700</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>1400</v>
+      </c>
+      <c r="I16" t="s">
+        <v>92</v>
+      </c>
+      <c r="M16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>100</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="I17" t="s">
+        <v>86</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="M17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>100</v>
+      </c>
+      <c r="E18">
+        <f t="shared" ref="E18" si="2">D18*C18</f>
+        <v>100</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <f t="shared" ref="G18" si="3">F18*E18</f>
+        <v>100</v>
+      </c>
+      <c r="I18" t="s">
+        <v>86</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="M18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>150</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+      <c r="I19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>50</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I20" t="s">
+        <v>86</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="M20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>150</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
+      <c r="I21" t="s">
+        <v>86</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="M21" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>200</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>400</v>
+      </c>
+      <c r="I22" t="s">
+        <v>92</v>
+      </c>
+      <c r="M22" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>100</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>50</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>100</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>50</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="M26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>99</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>100</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>108</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>140</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="1"/>
+        <v>140</v>
+      </c>
+      <c r="I30" t="s">
+        <v>86</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="M30" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <f t="shared" ref="E38:E45" si="4">D38*C38</f>
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <f t="shared" ref="G38:G45" si="5">F38*E38</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E46">
+        <f>SUM(E3:E45)</f>
+        <v>4690</v>
+      </c>
+      <c r="G46">
+        <f>SUM(G3:G45)</f>
+        <v>6840</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="M5" r:id="rId1"/>
+    <hyperlink ref="M6" r:id="rId2"/>
+    <hyperlink ref="M7" r:id="rId3"/>
+    <hyperlink ref="M8" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add power source 2 (eagle)
</commit_message>
<xml_diff>
--- a/doc/growmat_easy.xlsx
+++ b/doc/growmat_easy.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="24120" windowHeight="14460" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="24120" windowHeight="13005" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="price list" sheetId="2" r:id="rId1"/>
     <sheet name="growmat_easy_hydro" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" calcMode="manual" refMode="R1C1" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="112">
   <si>
     <t>box</t>
   </si>
@@ -345,6 +345,12 @@
   </si>
   <si>
     <t>https://www.postavrobota.cz/WiFi-RS232-AT-modul-ESP8266-2-4GHz-SoC-d159.htm</t>
+  </si>
+  <si>
+    <t>sim800l</t>
+  </si>
+  <si>
+    <t>http://www.ebay.com/itm/SIM800L-GPRS-GSM-SIM-Board-Quadband-QUAD-BAND-L-shape-Antenna-for-Arduino-/201647406545?hash=item2ef31f3dd1:g:-dgAAOSwZVlXsgXh</t>
   </si>
 </sst>
 </file>
@@ -1062,7 +1068,7 @@
   <dimension ref="A1:J97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1897,7 +1903,7 @@
   <dimension ref="B1:M46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2213,7 +2219,7 @@
       <c r="J11">
         <v>0</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M11" s="1" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2711,19 +2717,31 @@
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>110</v>
+      </c>
       <c r="C31">
         <v>1</v>
       </c>
+      <c r="D31">
+        <v>300</v>
+      </c>
       <c r="E31">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>D31*C31</f>
+        <v>300</v>
       </c>
       <c r="F31">
         <v>1</v>
       </c>
       <c r="G31">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>F31*E31</f>
+        <v>300</v>
+      </c>
+      <c r="I31" t="s">
+        <v>92</v>
+      </c>
+      <c r="M31" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.2">
@@ -2953,11 +2971,11 @@
     <row r="46" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E46">
         <f>SUM(E3:E45)</f>
-        <v>4690</v>
+        <v>4990</v>
       </c>
       <c r="G46">
         <f>SUM(G3:G45)</f>
-        <v>6840</v>
+        <v>7140</v>
       </c>
     </row>
   </sheetData>
@@ -2966,6 +2984,7 @@
     <hyperlink ref="M6" r:id="rId2"/>
     <hyperlink ref="M7" r:id="rId3"/>
     <hyperlink ref="M8" r:id="rId4"/>
+    <hyperlink ref="M11" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>